<commit_message>
changing saving tree structure 2025-05-11
</commit_message>
<xml_diff>
--- a/Individuell inlämningsuppgift/Inlämning_Erik_Unevik/vaderdata_ErikUnevik.xlsx
+++ b/Individuell inlämningsuppgift/Inlämning_Erik_Unevik/vaderdata_ErikUnevik.xlsx
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -489,14 +489,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-10-20</t>
+          <t>2025-05-11</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
-        <v>12.2</v>
+        <v>12.4</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -510,7 +510,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -521,14 +521,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-10-20</t>
+          <t>2025-05-11</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F3" t="n">
-        <v>12</v>
+        <v>13.3</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -542,7 +542,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -553,14 +553,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-10-20</t>
+          <t>2025-05-11</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F4" t="n">
-        <v>11.9</v>
+        <v>12.5</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -574,7 +574,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -585,14 +585,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-10-20</t>
+          <t>2025-05-11</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F5" t="n">
-        <v>11.9</v>
+        <v>12.4</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -606,7 +606,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -617,14 +617,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-10-20</t>
+          <t>2025-05-11</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F6" t="n">
-        <v>11.8</v>
+        <v>12</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -638,7 +638,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -649,14 +649,14 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-10-20</t>
+          <t>2025-05-11</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F7" t="n">
-        <v>11.7</v>
+        <v>11.2</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -670,7 +670,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -681,14 +681,14 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-10-20</t>
+          <t>2025-05-11</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F8" t="n">
-        <v>11.9</v>
+        <v>9.6</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -702,7 +702,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -713,14 +713,14 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-11</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F9" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -734,7 +734,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -745,14 +745,14 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-11</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F10" t="n">
-        <v>11.9</v>
+        <v>6.8</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -766,7 +766,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -777,14 +777,14 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-11</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="F11" t="n">
-        <v>12</v>
+        <v>6.1</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
@@ -798,7 +798,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -809,14 +809,14 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-11</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="F12" t="n">
-        <v>12</v>
+        <v>5.9</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
@@ -830,7 +830,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -841,17 +841,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>12</v>
+        <v>5.4</v>
       </c>
       <c r="G13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -862,7 +862,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -873,17 +873,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F14" t="n">
-        <v>12.2</v>
+        <v>4.7</v>
       </c>
       <c r="G14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -894,7 +894,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -905,17 +905,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F15" t="n">
-        <v>12.3</v>
+        <v>4.6</v>
       </c>
       <c r="G15" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -926,7 +926,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -937,17 +937,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F16" t="n">
-        <v>12.5</v>
+        <v>4.3</v>
       </c>
       <c r="G16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -958,7 +958,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -969,14 +969,14 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F17" t="n">
-        <v>13.2</v>
+        <v>6.1</v>
       </c>
       <c r="G17" t="b">
         <v>0</v>
@@ -990,7 +990,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1001,14 +1001,14 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E18" t="n">
+        <v>5</v>
+      </c>
+      <c r="F18" t="n">
         <v>9</v>
-      </c>
-      <c r="F18" t="n">
-        <v>13.9</v>
       </c>
       <c r="G18" t="b">
         <v>0</v>
@@ -1022,7 +1022,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1033,14 +1033,14 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F19" t="n">
-        <v>14.5</v>
+        <v>10.3</v>
       </c>
       <c r="G19" t="b">
         <v>0</v>
@@ -1054,7 +1054,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1065,14 +1065,14 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F20" t="n">
-        <v>14.8</v>
+        <v>11.1</v>
       </c>
       <c r="G20" t="b">
         <v>0</v>
@@ -1086,7 +1086,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1097,14 +1097,14 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F21" t="n">
-        <v>15.1</v>
+        <v>11.7</v>
       </c>
       <c r="G21" t="b">
         <v>0</v>
@@ -1118,7 +1118,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1129,14 +1129,14 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F22" t="n">
-        <v>14.7</v>
+        <v>11.9</v>
       </c>
       <c r="G22" t="b">
         <v>0</v>
@@ -1150,7 +1150,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1161,14 +1161,14 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F23" t="n">
-        <v>14.5</v>
+        <v>12.7</v>
       </c>
       <c r="G23" t="b">
         <v>0</v>
@@ -1182,7 +1182,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1193,14 +1193,14 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F24" t="n">
-        <v>14.1</v>
+        <v>14.2</v>
       </c>
       <c r="G24" t="b">
         <v>0</v>
@@ -1214,7 +1214,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1225,14 +1225,14 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F25" t="n">
-        <v>13.8</v>
+        <v>14.9</v>
       </c>
       <c r="G25" t="b">
         <v>0</v>
@@ -1246,7 +1246,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1257,14 +1257,14 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F26" t="n">
-        <v>13.5</v>
+        <v>14.9</v>
       </c>
       <c r="G26" t="b">
         <v>0</v>
@@ -1278,7 +1278,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2024-10-20 16:40</t>
+          <t>2025-05-11 13:16</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1289,14 +1289,14 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2024-10-21</t>
+          <t>2025-05-12</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F27" t="n">
-        <v>13.2</v>
+        <v>15.1</v>
       </c>
       <c r="G27" t="b">
         <v>0</v>

</xml_diff>